<commit_message>
Changed template and added more cell styling and data.
</commit_message>
<xml_diff>
--- a/templates/Prijevoz.xlsx
+++ b/templates/Prijevoz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\admin\admin\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B6BE5DE-A1F4-4719-A8D7-22794651D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80264301-1196-4729-A709-FA52465D70D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47CC8564-E4D4-4CB1-B47B-BFE93F75A985}"/>
+    <workbookView xWindow="3195" yWindow="2370" windowWidth="21600" windowHeight="11385" xr2:uid="{47CC8564-E4D4-4CB1-B47B-BFE93F75A985}"/>
   </bookViews>
   <sheets>
     <sheet name="obrazac" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Broj prijeđenih kilometara pri dolasku</t>
   </si>
@@ -59,24 +59,15 @@
     <t>PRI DOLASKU NA POSAO I ODLASKU S POSLA</t>
   </si>
   <si>
-    <t>Odobreni iznos za isplatu _______________ kn</t>
-  </si>
-  <si>
     <t>Na ime naknade troška prijevoza potražujem:</t>
   </si>
   <si>
-    <t>Naknada po prijeđenom kilometru:</t>
-  </si>
-  <si>
     <t>(potpis zaposlenika)</t>
   </si>
   <si>
     <t>(za Školu odobrava)</t>
   </si>
   <si>
-    <t>kn (stavak 6. ili st.8. čl. 67.)</t>
-  </si>
-  <si>
     <t>Za točnost i istinitost podataka iz ovog izvješća zaposlenik jamči potpisom pod punom krivičnom i materijalnom odgovornošću.</t>
   </si>
   <si>
@@ -84,78 +75,6 @@
   </si>
   <si>
     <t>UKUPNO:</t>
-  </si>
-  <si>
-    <t>1-</t>
-  </si>
-  <si>
-    <t>2-</t>
-  </si>
-  <si>
-    <t>3-</t>
-  </si>
-  <si>
-    <t>4-</t>
-  </si>
-  <si>
-    <t>5-</t>
-  </si>
-  <si>
-    <t>6-</t>
-  </si>
-  <si>
-    <t>7-</t>
-  </si>
-  <si>
-    <t>8-</t>
-  </si>
-  <si>
-    <t>9-</t>
-  </si>
-  <si>
-    <t>10-</t>
-  </si>
-  <si>
-    <t>11-</t>
-  </si>
-  <si>
-    <t>12-</t>
-  </si>
-  <si>
-    <t>13-</t>
-  </si>
-  <si>
-    <t>14-</t>
-  </si>
-  <si>
-    <t>15-</t>
-  </si>
-  <si>
-    <t>16-</t>
-  </si>
-  <si>
-    <t>17-</t>
-  </si>
-  <si>
-    <t>18-</t>
-  </si>
-  <si>
-    <t>19-</t>
-  </si>
-  <si>
-    <t>20-</t>
-  </si>
-  <si>
-    <t>21-</t>
-  </si>
-  <si>
-    <t>22-</t>
-  </si>
-  <si>
-    <t>23-</t>
-  </si>
-  <si>
-    <t>24-</t>
   </si>
   <si>
     <t>Adresa rada: Ilok, Matije Gupca 168</t>
@@ -169,6 +88,9 @@
   <si>
     <t>Datum 
  mjesec SIJEČANJ -  2022</t>
+  </si>
+  <si>
+    <t>Odobreni iznos za isplatu _______________ EUR</t>
   </si>
 </sst>
 </file>
@@ -306,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -320,9 +242,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,28 +258,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -371,13 +286,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A76C778-8189-4AED-878B-6CD3A66769FF}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,57 +616,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="A3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>43</v>
+      <c r="A5" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>0</v>
@@ -764,298 +682,248 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10" s="15"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>18</v>
-      </c>
+      <c r="A11" s="15"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>19</v>
-      </c>
+      <c r="A12" s="15"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="15"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="15"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="5">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="16"/>
+      <c r="B33" s="18">
         <v>1</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="17">
         <v>2</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="25"/>
-    </row>
-    <row r="34" spans="1:5" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="11">
+      <c r="E33" s="22"/>
+    </row>
+    <row r="34" spans="1:5" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="10">
         <f>SUM(B10:B32)</f>
         <v>0</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10">
         <f>SUM(C10:C32)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D34" s="23">
         <f>SUM(B34:C34)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="26"/>
+      <c r="E34" s="23"/>
     </row>
     <row r="36" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
+      <c r="A36" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+    <row r="38" spans="1:5" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+    </row>
+    <row r="39" spans="1:5" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:5" s="13" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:5" s="13" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D41" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="20"/>
+    </row>
+    <row r="42" spans="1:5" s="13" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:5" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="13" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D44" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="18"/>
-    </row>
-    <row r="40" spans="1:5" s="17" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:5" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="D41" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="23"/>
-    </row>
-    <row r="42" spans="1:5" s="17" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="D44" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="23"/>
-    </row>
-    <row r="45" spans="1:5" s="17" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="8"/>
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="1:5" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D45" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D44:E44"/>
@@ -1064,6 +932,7 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A38:E38"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>